<commit_message>
Updated templates for tests and removed test for removed code.
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Normalization_planning_v4_4_0_Library.xlsx
+++ b/backend/fms_core/tests/valid_templates/Normalization_planning_v4_4_0_Library.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t xml:space="preserve">Sample and Library Normalization Planning Template</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t xml:space="preserve">Source Container Coord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source Container Location Barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source Container Location Coord</t>
   </si>
   <si>
     <t xml:space="preserve">Destination Container Barcode</t>
@@ -695,7 +701,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P1002"/>
+  <dimension ref="A1:R1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -703,7 +709,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.86"/>
@@ -758,22 +764,24 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -793,13 +801,13 @@
       <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -808,16 +816,16 @@
       <c r="J5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="9" t="s">
         <v>20</v>
       </c>
       <c r="O5" s="7" t="s">
@@ -826,118 +834,130 @@
       <c r="P5" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="Q5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="I6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="N6" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="Q6" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="R6" s="0" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="H7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="0" t="n">
+      <c r="M7" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="N7" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="Q7" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="P7" s="0" t="n">
+      <c r="R7" s="0" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="N8" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="Q8" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="P8" s="0" t="n">
+      <c r="R8" s="0" t="n">
         <v>50</v>
       </c>
     </row>
@@ -7682,7 +7702,7 @@
       <formula1>Info!$B$2:$B$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H8" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J8" type="list">
       <formula1>Info!$A$2:$A$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7708,46 +7728,46 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7756,7 +7776,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C11" s="18"/>
     </row>
@@ -7765,7 +7785,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C12" s="18"/>
     </row>
@@ -7774,7 +7794,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C13" s="18"/>
     </row>
@@ -7783,115 +7803,115 @@
         <v>10</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C19" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C20" s="18"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C22" s="18"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C23" s="18"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C24" s="18"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C25" s="18"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C26" s="18"/>
     </row>
@@ -7918,7 +7938,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
@@ -7929,60 +7949,60 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>